<commit_message>
updaed for 24th week
</commit_message>
<xml_diff>
--- a/plan/plan_tracklist.xlsx
+++ b/plan/plan_tracklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715"/>
@@ -18,10 +18,113 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>unicornx</author>
     <author>Administrator</author>
   </authors>
   <commentList>
-    <comment ref="E8" authorId="0">
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>unicornx:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>目前以</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> linuxlab</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">系列为主
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>unicornx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>目前以</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> shell </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">编程系列
+为主
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -55,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F10" authorId="1">
       <text>
         <r>
           <rPr>
@@ -89,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -123,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0">
+    <comment ref="F12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -157,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -191,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -225,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0">
+    <comment ref="F15" authorId="1">
       <text>
         <r>
           <rPr>
@@ -259,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0">
+    <comment ref="F16" authorId="1">
       <text>
         <r>
           <rPr>
@@ -298,7 +401,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Sunday</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1549,178 +1652,6 @@
   </si>
   <si>
     <t>欢迎投稿</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>利用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Linux Lab </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>完成嵌入式系统软件开发全过程</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Docker/Qemu </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>快速构建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Linux </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>内核实验环境</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>五分钟内搭建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Linux 0.11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的实验环境</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>基于</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Docker </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>快速构建</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Linux 0.11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>实验环境</t>
-    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1905,6 +1836,96 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>lwn 117749: 4 level page tables merged</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shell </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>编程范例</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）进程操作</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>lwn 415740: tty-based group scheduling</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Linux Lab </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>发布</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> v0.1 rc1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>[</t>
     </r>
@@ -1991,67 +2012,313 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>lwn 117749: 4 level page tables merged</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Shell </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>编程范例</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）进程操作</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lwn 415740: tty-based group scheduling</t>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>泰晓资讯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>·06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>月</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>期</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> / 2019]</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bugfix: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>消除</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> qemu/raspi3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启动过程的一堆警告</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(2019-06-11-00-41-33-bugfix-silence-raspi3-boot-warnings.md)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bugfix: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> git bisect </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>自动定位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> uboot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>启动失败问题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(2019-06-11-02-59-23-bugfix-git-bisect-uboot-failure.md)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Linux Lab </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>新开发板添加指南</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(2019-06-11-07-01-41-add-new-board-for-linux-lab.md)</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>泰晓资讯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>·06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>月</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>期</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> / 2019]</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2059,7 +2326,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2145,8 +2412,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2168,12 +2443,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2215,7 +2484,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2244,9 +2513,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2550,7 +2816,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2585,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>38</v>
@@ -2612,7 +2878,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="28.5">
@@ -2636,7 +2902,7 @@
         <v>54</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="84.75">
@@ -2648,7 +2914,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>8</v>
@@ -2657,10 +2923,10 @@
         <v>41</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="28.5">
@@ -2672,7 +2938,7 @@
         <v>36</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>9</v>
@@ -2684,35 +2950,38 @@
         <v>72</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.5">
       <c r="A6" s="3">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>55</v>
+      <c r="C6" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="G6" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="H6" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5">
+    <row r="7" spans="1:8" ht="71.25">
       <c r="A7" s="3">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>56</v>
+      <c r="C7" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -2721,39 +2990,36 @@
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>50</v>
+        <v>75</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.5">
+    <row r="8" spans="1:8" ht="57">
       <c r="A8" s="3">
         <v>26</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="3">
         <v>27</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
@@ -2761,10 +3027,10 @@
         <v>53</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.5">
@@ -2774,11 +3040,11 @@
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>46</v>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.5">
@@ -2788,8 +3054,8 @@
       <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
+      <c r="F11" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5">
@@ -2799,8 +3065,8 @@
       <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>47</v>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5">
@@ -2811,7 +3077,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.5">
@@ -2821,16 +3087,19 @@
       <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>51</v>
+      <c r="F14" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="28.5">
       <c r="A15" s="3">
         <v>33</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2839,6 +3108,9 @@
       </c>
       <c r="D16" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28.5">

</xml_diff>